<commit_message>
two stage GA optimization implemented
</commit_message>
<xml_diff>
--- a/targets_RVE_1_40_D/exp_curveDB.xlsx
+++ b/targets_RVE_1_40_D/exp_curveDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaltofi.sharepoint.com/sites/LianGroup-CPparameteroptimization/Shared Documents/CP parameter optimization/02 Reference for CSC/DB material(RVE3615Grains)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Desktop\Crystal-Plasticity-Project\targets_RVE_1_40_D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_5F89156F0B8BCEC08E8F1BED38C33D29F4204EC6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CB1A58A-EEA3-4CE1-A03F-82FF25C9EA10}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127BE12A-B54D-42E5-99DC-6FF952190A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-110" windowWidth="24630" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB3615" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="38">
   <si>
     <t>DB3615_1</t>
   </si>
@@ -119,12 +119,42 @@
   <si>
     <t>[100-200]</t>
   </si>
+  <si>
+    <t>DB1</t>
+  </si>
+  <si>
+    <t>stage 1: fit yeild points</t>
+  </si>
+  <si>
+    <t>stage 2: Hardening parameter</t>
+  </si>
+  <si>
+    <t>[0.05-3]</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[5-500]</t>
+  </si>
+  <si>
+    <t>[1-25]</t>
+  </si>
+  <si>
+    <t>DB2</t>
+  </si>
+  <si>
+    <t>[0.1-10]</t>
+  </si>
+  <si>
+    <t>DB3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,13 +162,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,9 +202,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1709,7 +1768,7 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="600474816"/>
@@ -1762,7 +1821,7 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-FI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="600474400"/>
@@ -1810,7 +1869,7 @@
           <a:latin typeface="+mn-lt"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-FI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2127,18 +2186,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457D16A4-B188-401F-AF85-44B5CAA7A197}">
-  <dimension ref="H1:X83"/>
+  <dimension ref="H1:AF83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="28" max="28" width="21.21875" customWidth="1"/>
+    <col min="29" max="29" width="16.109375" customWidth="1"/>
+    <col min="30" max="30" width="29" customWidth="1"/>
+    <col min="31" max="31" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I1" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="8:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I2" t="s">
         <v>3</v>
       </c>
@@ -2187,7 +2250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="8:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="8:32" x14ac:dyDescent="0.3">
       <c r="H3" t="s">
         <v>7</v>
       </c>
@@ -2219,7 +2282,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="8:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="8:32" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
         <v>9</v>
       </c>
@@ -2250,8 +2313,20 @@
       <c r="W4">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="5" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="2"/>
+    </row>
+    <row r="5" spans="8:32" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
         <v>11</v>
       </c>
@@ -2282,8 +2357,22 @@
       <c r="W5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="6" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="2"/>
+    </row>
+    <row r="6" spans="8:32" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
         <v>13</v>
       </c>
@@ -2314,8 +2403,24 @@
       <c r="W6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF6" s="2"/>
+    </row>
+    <row r="7" spans="8:32" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
         <v>15</v>
       </c>
@@ -2346,8 +2451,24 @@
       <c r="W7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF7" s="2"/>
+    </row>
+    <row r="8" spans="8:32" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
         <v>18</v>
       </c>
@@ -2378,8 +2499,40 @@
       <c r="W8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF8" s="2"/>
+    </row>
+    <row r="9" spans="8:32" x14ac:dyDescent="0.3">
+      <c r="AA9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>80</v>
+      </c>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="2"/>
+    </row>
+    <row r="10" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
         <v>19</v>
       </c>
@@ -2398,8 +2551,22 @@
       <c r="W10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="2"/>
+    </row>
+    <row r="11" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I11" s="1">
         <v>1.69673711605E-7</v>
       </c>
@@ -2414,7 +2581,7 @@
         <v>1.69673711605E-7</v>
       </c>
       <c r="P11" s="1">
-        <f>O11/1000000</f>
+        <f t="shared" ref="P11:P42" si="1">O11/1000000</f>
         <v>1.6967371160500001E-13</v>
       </c>
       <c r="Q11">
@@ -2425,15 +2592,29 @@
         <v>1.69673711605E-7</v>
       </c>
       <c r="V11" s="1">
-        <f t="shared" ref="V11:V42" si="1">U11/1000000</f>
+        <f t="shared" ref="V11:V42" si="2">U11/1000000</f>
         <v>1.6967371160500001E-13</v>
       </c>
       <c r="W11">
         <v>0</v>
       </c>
       <c r="X11" s="1"/>
-    </row>
-    <row r="12" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="2"/>
+    </row>
+    <row r="12" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I12">
         <v>14171348.608899999</v>
       </c>
@@ -2448,7 +2629,7 @@
         <v>14171348.608899999</v>
       </c>
       <c r="P12" s="1">
-        <f>O12/1000000</f>
+        <f t="shared" si="1"/>
         <v>14.171348608899999</v>
       </c>
       <c r="Q12">
@@ -2458,14 +2639,20 @@
         <v>14171348.608899999</v>
       </c>
       <c r="V12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.171348608899999</v>
       </c>
       <c r="W12">
         <v>1.7761643412099999E-4</v>
       </c>
-    </row>
-    <row r="13" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+    </row>
+    <row r="13" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I13">
         <v>28354970.570500001</v>
       </c>
@@ -2480,7 +2667,7 @@
         <v>28354970.570500001</v>
       </c>
       <c r="P13" s="1">
-        <f>O13/1000000</f>
+        <f t="shared" si="1"/>
         <v>28.354970570500001</v>
       </c>
       <c r="Q13">
@@ -2490,14 +2677,20 @@
         <v>28354970.570500001</v>
       </c>
       <c r="V13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.354970570500001</v>
       </c>
       <c r="W13">
         <v>3.5522096588900003E-4</v>
       </c>
-    </row>
-    <row r="14" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+    </row>
+    <row r="14" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I14">
         <v>42550873.612300001</v>
       </c>
@@ -2512,7 +2705,7 @@
         <v>42550873.612400003</v>
       </c>
       <c r="P14" s="1">
-        <f>O14/1000000</f>
+        <f t="shared" si="1"/>
         <v>42.550873612400004</v>
       </c>
       <c r="Q14">
@@ -2522,14 +2715,26 @@
         <v>42550873.612300001</v>
       </c>
       <c r="V14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42.550873612300002</v>
       </c>
       <c r="W14">
         <v>5.3281361137699995E-4</v>
       </c>
-    </row>
-    <row r="15" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="2"/>
+    </row>
+    <row r="15" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I15">
         <v>54068782.000399999</v>
       </c>
@@ -2544,7 +2749,7 @@
         <v>56700028.137900002</v>
       </c>
       <c r="P15" s="1">
-        <f>O15/1000000</f>
+        <f t="shared" si="1"/>
         <v>56.700028137900006</v>
       </c>
       <c r="Q15">
@@ -2554,14 +2759,28 @@
         <v>56759065.468099996</v>
       </c>
       <c r="V15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56.759065468099998</v>
       </c>
       <c r="W15">
         <v>7.1039438598199999E-4</v>
       </c>
-    </row>
-    <row r="16" spans="8:24" x14ac:dyDescent="0.35">
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF15" s="2"/>
+    </row>
+    <row r="16" spans="8:32" x14ac:dyDescent="0.3">
       <c r="I16">
         <v>58620201.260200001</v>
       </c>
@@ -2576,7 +2795,7 @@
         <v>69976823.361300007</v>
       </c>
       <c r="P16" s="1">
-        <f>O16/1000000</f>
+        <f t="shared" si="1"/>
         <v>69.976823361300006</v>
       </c>
       <c r="Q16">
@@ -2586,14 +2805,30 @@
         <v>70979553.877599999</v>
       </c>
       <c r="V16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70.979553877599997</v>
       </c>
       <c r="W16">
         <v>8.8796330576900004E-4</v>
       </c>
-    </row>
-    <row r="17" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF16" s="2"/>
+    </row>
+    <row r="17" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I17">
         <v>61198767.651900001</v>
       </c>
@@ -2608,7 +2843,7 @@
         <v>80823823.120000005</v>
       </c>
       <c r="P17" s="1">
-        <f>O17/1000000</f>
+        <f t="shared" si="1"/>
         <v>80.82382312</v>
       </c>
       <c r="Q17">
@@ -2618,14 +2853,30 @@
         <v>85212346.586799994</v>
       </c>
       <c r="V17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>85.212346586799995</v>
       </c>
       <c r="W17">
         <v>1.06552038646E-3</v>
       </c>
-    </row>
-    <row r="18" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF17" s="2"/>
+    </row>
+    <row r="18" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I18">
         <v>63140223.2346</v>
       </c>
@@ -2640,7 +2891,7 @@
         <v>88574620.228300005</v>
       </c>
       <c r="P18" s="1">
-        <f>O18/1000000</f>
+        <f t="shared" si="1"/>
         <v>88.574620228300006</v>
       </c>
       <c r="Q18">
@@ -2650,14 +2901,30 @@
         <v>99457278.205899999</v>
       </c>
       <c r="V18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.457278205899996</v>
       </c>
       <c r="W18">
         <v>1.24306591277E-3</v>
       </c>
-    </row>
-    <row r="19" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF18" s="2"/>
+    </row>
+    <row r="19" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I19">
         <v>64724225.130099997</v>
       </c>
@@ -2672,7 +2939,7 @@
         <v>93740188.221000001</v>
       </c>
       <c r="P19" s="1">
-        <f>O19/1000000</f>
+        <f t="shared" si="1"/>
         <v>93.740188220999997</v>
       </c>
       <c r="Q19">
@@ -2682,14 +2949,28 @@
         <v>113713191.14300001</v>
       </c>
       <c r="V19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.713191143</v>
       </c>
       <c r="W19">
         <v>1.42060170763E-3</v>
       </c>
-    </row>
-    <row r="20" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" s="5">
+        <v>80</v>
+      </c>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF19" s="2"/>
+    </row>
+    <row r="20" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I20">
         <v>66060252.291199997</v>
       </c>
@@ -2704,7 +2985,7 @@
         <v>97163428.922700003</v>
       </c>
       <c r="P20" s="1">
-        <f>O20/1000000</f>
+        <f t="shared" si="1"/>
         <v>97.163428922700007</v>
       </c>
       <c r="Q20">
@@ -2714,14 +2995,28 @@
         <v>127977357.331</v>
       </c>
       <c r="V20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127.97735733099999</v>
       </c>
       <c r="W20">
         <v>1.5981320090799999E-3</v>
       </c>
-    </row>
-    <row r="21" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE20" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AF20" s="2"/>
+    </row>
+    <row r="21" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I21">
         <v>67222886.221000001</v>
       </c>
@@ -2736,7 +3031,7 @@
         <v>99509143.060699999</v>
       </c>
       <c r="P21" s="1">
-        <f>O21/1000000</f>
+        <f t="shared" si="1"/>
         <v>99.509143060699998</v>
       </c>
       <c r="Q21">
@@ -2746,14 +3041,28 @@
         <v>142241164.83199999</v>
       </c>
       <c r="V21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>142.24116483199998</v>
       </c>
       <c r="W21">
         <v>1.77567010979E-3</v>
       </c>
-    </row>
-    <row r="22" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE21" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AF21" s="2"/>
+    </row>
+    <row r="22" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I22">
         <v>68267667.814799994</v>
       </c>
@@ -2768,7 +3077,7 @@
         <v>101194750.464</v>
       </c>
       <c r="P22" s="1">
-        <f>O22/1000000</f>
+        <f t="shared" si="1"/>
         <v>101.19475046399999</v>
       </c>
       <c r="Q22">
@@ -2778,14 +3087,20 @@
         <v>156478028.162</v>
       </c>
       <c r="V22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156.47802816199999</v>
       </c>
       <c r="W22">
         <v>1.9532569031700002E-3</v>
       </c>
-    </row>
-    <row r="23" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+    </row>
+    <row r="23" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I23">
         <v>69232544.717999995</v>
       </c>
@@ -2800,7 +3115,7 @@
         <v>102462143.072</v>
       </c>
       <c r="P23" s="1">
-        <f>O23/1000000</f>
+        <f t="shared" si="1"/>
         <v>102.462143072</v>
       </c>
       <c r="Q23">
@@ -2810,14 +3125,20 @@
         <v>170610146.41600001</v>
       </c>
       <c r="V23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>170.61014641600002</v>
       </c>
       <c r="W23">
         <v>2.1310117375500002E-3</v>
       </c>
-    </row>
-    <row r="24" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+    </row>
+    <row r="24" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I24">
         <v>70141514.797399998</v>
       </c>
@@ -2832,7 +3153,7 @@
         <v>103450610.52</v>
       </c>
       <c r="P24" s="1">
-        <f>O24/1000000</f>
+        <f t="shared" si="1"/>
         <v>103.45061052</v>
       </c>
       <c r="Q24">
@@ -2842,14 +3163,26 @@
         <v>184428741.491</v>
       </c>
       <c r="V24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184.42874149099998</v>
       </c>
       <c r="W24">
         <v>2.3092541417400001E-3</v>
       </c>
-    </row>
-    <row r="25" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="2"/>
+    </row>
+    <row r="25" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I25">
         <v>71010598.089300007</v>
       </c>
@@ -2864,7 +3197,7 @@
         <v>104243522.588</v>
       </c>
       <c r="P25" s="1">
-        <f>O25/1000000</f>
+        <f t="shared" si="1"/>
         <v>104.243522588</v>
       </c>
       <c r="Q25">
@@ -2874,14 +3207,28 @@
         <v>197467668.699</v>
       </c>
       <c r="V25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>197.467668699</v>
       </c>
       <c r="W25">
         <v>2.48869602136E-3</v>
       </c>
-    </row>
-    <row r="26" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF25" s="2"/>
+    </row>
+    <row r="26" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I26">
         <v>71849963.886899993</v>
       </c>
@@ -2896,7 +3243,7 @@
         <v>104894018.469</v>
       </c>
       <c r="P26" s="1">
-        <f>O26/1000000</f>
+        <f t="shared" si="1"/>
         <v>104.894018469</v>
       </c>
       <c r="Q26">
@@ -2906,14 +3253,30 @@
         <v>208997181.42699999</v>
       </c>
       <c r="V26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>208.99718142699999</v>
       </c>
       <c r="W26">
         <v>2.6704499970499999E-3</v>
       </c>
-    </row>
-    <row r="27" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF26" s="2"/>
+    </row>
+    <row r="27" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I27">
         <v>72666153.2984</v>
       </c>
@@ -2928,7 +3291,7 @@
         <v>105438285.788</v>
       </c>
       <c r="P27" s="1">
-        <f>O27/1000000</f>
+        <f t="shared" si="1"/>
         <v>105.438285788</v>
       </c>
       <c r="Q27">
@@ -2938,14 +3301,30 @@
         <v>218396826.08500001</v>
       </c>
       <c r="V27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>218.39682608500001</v>
       </c>
       <c r="W27">
         <v>2.85546238859E-3</v>
       </c>
-    </row>
-    <row r="28" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF27" s="2"/>
+    </row>
+    <row r="28" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I28">
         <v>73463920.8917</v>
       </c>
@@ -2960,7 +3339,7 @@
         <v>105902348.971</v>
       </c>
       <c r="P28" s="1">
-        <f>O28/1000000</f>
+        <f t="shared" si="1"/>
         <v>105.902348971</v>
       </c>
       <c r="Q28">
@@ -2970,14 +3349,30 @@
         <v>225591864.17399999</v>
       </c>
       <c r="V28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>225.59186417399999</v>
       </c>
       <c r="W28">
         <v>3.0438536624499998E-3</v>
       </c>
-    </row>
-    <row r="29" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC28" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="AD28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF28" s="2"/>
+    </row>
+    <row r="29" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I29">
         <v>74246737.265400007</v>
       </c>
@@ -2992,7 +3387,7 @@
         <v>106305634.426</v>
       </c>
       <c r="P29" s="1">
-        <f>O29/1000000</f>
+        <f t="shared" si="1"/>
         <v>106.305634426</v>
       </c>
       <c r="Q29">
@@ -3002,14 +3397,28 @@
         <v>230981658.28099999</v>
       </c>
       <c r="V29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>230.98165828099999</v>
       </c>
       <c r="W29">
         <v>3.2350288371600002E-3</v>
       </c>
-    </row>
-    <row r="30" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB29" s="5">
+        <v>80</v>
+      </c>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE29" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF29" s="2"/>
+    </row>
+    <row r="30" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I30">
         <v>75017060.901899993</v>
       </c>
@@ -3024,7 +3433,7 @@
         <v>106662963.345</v>
       </c>
       <c r="P30" s="1">
-        <f>O30/1000000</f>
+        <f t="shared" si="1"/>
         <v>106.66296334499999</v>
       </c>
       <c r="Q30">
@@ -3034,14 +3443,28 @@
         <v>235083245.14899999</v>
       </c>
       <c r="V30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>235.08324514899999</v>
       </c>
       <c r="W30">
         <v>3.4282148959599999E-3</v>
       </c>
-    </row>
-    <row r="31" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB30" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE30" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF30" s="2"/>
+    </row>
+    <row r="31" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I31">
         <v>75776668.682600006</v>
       </c>
@@ -3056,7 +3479,7 @@
         <v>106985762.12100001</v>
       </c>
       <c r="P31" s="1">
-        <f>O31/1000000</f>
+        <f t="shared" si="1"/>
         <v>106.98576212100001</v>
       </c>
       <c r="Q31">
@@ -3066,14 +3489,28 @@
         <v>238315951.01699999</v>
       </c>
       <c r="V31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>238.315951017</v>
       </c>
       <c r="W31">
         <v>3.6227837414400002E-3</v>
       </c>
-    </row>
-    <row r="32" spans="9:23" x14ac:dyDescent="0.35">
+      <c r="AA31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB31" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE31" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF31" s="2"/>
+    </row>
+    <row r="32" spans="9:32" x14ac:dyDescent="0.3">
       <c r="I32">
         <v>77636811.511299998</v>
       </c>
@@ -3088,7 +3525,7 @@
         <v>107694899.47499999</v>
       </c>
       <c r="P32" s="1">
-        <f>O32/1000000</f>
+        <f t="shared" si="1"/>
         <v>107.694899475</v>
       </c>
       <c r="Q32">
@@ -3098,14 +3535,14 @@
         <v>244214957.79699999</v>
       </c>
       <c r="V32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>244.21495779699998</v>
       </c>
       <c r="W32">
         <v>4.1128122351099996E-3</v>
       </c>
     </row>
-    <row r="33" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I33">
         <v>79451710.503999993</v>
       </c>
@@ -3120,7 +3557,7 @@
         <v>108329839.145</v>
       </c>
       <c r="P33" s="1">
-        <f>O33/1000000</f>
+        <f t="shared" si="1"/>
         <v>108.32983914499999</v>
       </c>
       <c r="Q33">
@@ -3130,14 +3567,14 @@
         <v>248459413.986</v>
       </c>
       <c r="V33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>248.45941398600002</v>
       </c>
       <c r="W33">
         <v>4.6057261330300003E-3</v>
       </c>
     </row>
-    <row r="34" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I34">
         <v>81230298.023599997</v>
       </c>
@@ -3152,7 +3589,7 @@
         <v>108938116.954</v>
       </c>
       <c r="P34" s="1">
-        <f>O34/1000000</f>
+        <f t="shared" si="1"/>
         <v>108.93811695399999</v>
       </c>
       <c r="Q34">
@@ -3162,14 +3599,14 @@
         <v>251808635.66800001</v>
       </c>
       <c r="V34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>251.80863566800002</v>
       </c>
       <c r="W34">
         <v>5.1002678971700001E-3</v>
       </c>
     </row>
-    <row r="35" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I35">
         <v>82978087.085999995</v>
       </c>
@@ -3184,7 +3621,7 @@
         <v>109543630.84199999</v>
       </c>
       <c r="P35" s="1">
-        <f>O35/1000000</f>
+        <f t="shared" si="1"/>
         <v>109.543630842</v>
       </c>
       <c r="Q35">
@@ -3194,14 +3631,14 @@
         <v>254547687.20199999</v>
       </c>
       <c r="V35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>254.54768720199999</v>
       </c>
       <c r="W35">
         <v>5.5958874755000004E-3</v>
       </c>
     </row>
-    <row r="36" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I36">
         <v>84698571.672299996</v>
       </c>
@@ -3216,7 +3653,7 @@
         <v>110157804.85600001</v>
       </c>
       <c r="P36" s="1">
-        <f>O36/1000000</f>
+        <f t="shared" si="1"/>
         <v>110.15780485600001</v>
       </c>
       <c r="Q36">
@@ -3226,14 +3663,14 @@
         <v>256807646.63299999</v>
       </c>
       <c r="V36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>256.80764663299999</v>
       </c>
       <c r="W36">
         <v>6.0922760723700004E-3</v>
       </c>
     </row>
-    <row r="37" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I37">
         <v>86394364.148399994</v>
       </c>
@@ -3248,7 +3685,7 @@
         <v>110785561.552</v>
       </c>
       <c r="P37" s="1">
-        <f>O37/1000000</f>
+        <f t="shared" si="1"/>
         <v>110.785561552</v>
       </c>
       <c r="Q37">
@@ -3258,14 +3695,14 @@
         <v>258675097.97099999</v>
       </c>
       <c r="V37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>258.67509797100001</v>
       </c>
       <c r="W37">
         <v>6.5892099609999996E-3</v>
       </c>
     </row>
-    <row r="38" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I38">
         <v>88067615.982899994</v>
       </c>
@@ -3280,7 +3717,7 @@
         <v>111428459.93099999</v>
       </c>
       <c r="P38" s="1">
-        <f>O38/1000000</f>
+        <f t="shared" si="1"/>
         <v>111.42845993099999</v>
       </c>
       <c r="Q38">
@@ -3290,14 +3727,14 @@
         <v>260224895.36199999</v>
       </c>
       <c r="V38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>260.22489536199998</v>
       </c>
       <c r="W38">
         <v>7.0865047938800003E-3</v>
       </c>
     </row>
-    <row r="39" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I39">
         <v>89719876.606900007</v>
       </c>
@@ -3312,7 +3749,7 @@
         <v>112086349.51199999</v>
       </c>
       <c r="P39" s="1">
-        <f>O39/1000000</f>
+        <f t="shared" si="1"/>
         <v>112.086349512</v>
       </c>
       <c r="Q39">
@@ -3322,14 +3759,14 @@
         <v>261523907.78200001</v>
       </c>
       <c r="V39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>261.52390778199998</v>
       </c>
       <c r="W39">
         <v>7.5840068029700003E-3</v>
       </c>
     </row>
-    <row r="40" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I40">
         <v>91352432.036699995</v>
       </c>
@@ -3344,7 +3781,7 @@
         <v>112758251.024</v>
       </c>
       <c r="P40" s="1">
-        <f>O40/1000000</f>
+        <f t="shared" si="1"/>
         <v>112.758251024</v>
       </c>
       <c r="Q40">
@@ -3354,14 +3791,14 @@
         <v>262629010.03799999</v>
       </c>
       <c r="V40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>262.62901003799999</v>
       </c>
       <c r="W40">
         <v>8.0815917259700002E-3</v>
       </c>
     </row>
-    <row r="41" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I41">
         <v>92966412.139200002</v>
       </c>
@@ -3376,7 +3813,7 @@
         <v>113442820.323</v>
       </c>
       <c r="P41" s="1">
-        <f>O41/1000000</f>
+        <f t="shared" si="1"/>
         <v>113.44282032299999</v>
       </c>
       <c r="Q41">
@@ -3386,14 +3823,14 @@
         <v>263586021.21200001</v>
       </c>
       <c r="V41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>263.58602121199999</v>
       </c>
       <c r="W41">
         <v>8.5791638088100006E-3</v>
       </c>
     </row>
-    <row r="42" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I42">
         <v>94562786.9604</v>
       </c>
@@ -3408,7 +3845,7 @@
         <v>114138600.49699999</v>
       </c>
       <c r="P42" s="1">
-        <f>O42/1000000</f>
+        <f t="shared" si="1"/>
         <v>114.138600497</v>
       </c>
       <c r="Q42">
@@ -3418,19 +3855,19 @@
         <v>264430419.78799999</v>
       </c>
       <c r="V42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>264.43041978799999</v>
       </c>
       <c r="W42">
         <v>9.0766519259099995E-3</v>
       </c>
     </row>
-    <row r="43" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I43">
         <v>96142413.8706</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" ref="J43:J74" si="2">I43/1000000</f>
+        <f t="shared" ref="J43:J74" si="3">I43/1000000</f>
         <v>96.142413870599995</v>
       </c>
       <c r="K43">
@@ -3440,7 +3877,7 @@
         <v>114844154.08400001</v>
       </c>
       <c r="P43" s="1">
-        <f>O43/1000000</f>
+        <f t="shared" ref="P43:P74" si="4">O43/1000000</f>
         <v>114.84415408400001</v>
       </c>
       <c r="Q43">
@@ -3450,19 +3887,19 @@
         <v>265189072.55500001</v>
       </c>
       <c r="V43" s="1">
-        <f t="shared" ref="V43:V74" si="3">U43/1000000</f>
+        <f t="shared" ref="V43:V74" si="5">U43/1000000</f>
         <v>265.189072555</v>
       </c>
       <c r="W43">
         <v>9.5740041180900001E-3</v>
       </c>
     </row>
-    <row r="44" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I44">
         <v>97706060.578600004</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97.706060578600002</v>
       </c>
       <c r="K44">
@@ -3472,7 +3909,7 @@
         <v>115558125.417</v>
       </c>
       <c r="P44" s="1">
-        <f>O44/1000000</f>
+        <f t="shared" si="4"/>
         <v>115.558125417</v>
       </c>
       <c r="Q44">
@@ -3482,19 +3919,19 @@
         <v>265882129.47600001</v>
       </c>
       <c r="V44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>265.88212947599999</v>
       </c>
       <c r="W44">
         <v>1.00711828719E-2</v>
       </c>
     </row>
-    <row r="45" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I45">
         <v>99254436.260100007</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99.254436260100007</v>
       </c>
       <c r="K45">
@@ -3504,7 +3941,7 @@
         <v>116279271.63699999</v>
       </c>
       <c r="P45" s="1">
-        <f>O45/1000000</f>
+        <f t="shared" si="4"/>
         <v>116.27927163699999</v>
       </c>
       <c r="Q45">
@@ -3514,19 +3951,19 @@
         <v>266524680.574</v>
       </c>
       <c r="V45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>266.524680574</v>
       </c>
       <c r="W45">
         <v>1.05681614635E-2</v>
       </c>
     </row>
-    <row r="46" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I46">
         <v>100788193.292</v>
       </c>
       <c r="J46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100.788193292</v>
       </c>
       <c r="K46">
@@ -3536,7 +3973,7 @@
         <v>117006468.602</v>
       </c>
       <c r="P46" s="1">
-        <f>O46/1000000</f>
+        <f t="shared" si="4"/>
         <v>117.006468602</v>
       </c>
       <c r="Q46">
@@ -3546,19 +3983,19 @@
         <v>267128052.243</v>
       </c>
       <c r="V46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>267.12805224300001</v>
       </c>
       <c r="W46">
         <v>1.10649210599E-2</v>
       </c>
     </row>
-    <row r="47" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I47">
         <v>102307917.221</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102.307917221</v>
       </c>
       <c r="K47">
@@ -3568,7 +4005,7 @@
         <v>117738710.311</v>
       </c>
       <c r="P47" s="1">
-        <f>O47/1000000</f>
+        <f t="shared" si="4"/>
         <v>117.73871031100001</v>
       </c>
       <c r="Q47">
@@ -3578,19 +4015,19 @@
         <v>267700779.664</v>
       </c>
       <c r="V47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>267.70077966399998</v>
       </c>
       <c r="W47">
         <v>1.1561448483600001E-2</v>
       </c>
     </row>
-    <row r="48" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I48">
         <v>103814134.54099999</v>
       </c>
       <c r="J48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>103.81413454099999</v>
       </c>
       <c r="K48">
@@ -3600,7 +4037,7 @@
         <v>118475098.286</v>
       </c>
       <c r="P48" s="1">
-        <f>O48/1000000</f>
+        <f t="shared" si="4"/>
         <v>118.47509828600001</v>
       </c>
       <c r="Q48">
@@ -3610,19 +4047,19 @@
         <v>268249324.87799999</v>
       </c>
       <c r="V48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>268.24932487799998</v>
       </c>
       <c r="W48">
         <v>1.20577345628E-2</v>
       </c>
     </row>
-    <row r="49" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="49" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I49">
         <v>105307327.42</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>105.30732742000001</v>
       </c>
       <c r="K49">
@@ -3632,7 +4069,7 @@
         <v>119214837.04899999</v>
       </c>
       <c r="P49" s="1">
-        <f>O49/1000000</f>
+        <f t="shared" si="4"/>
         <v>119.214837049</v>
       </c>
       <c r="Q49">
@@ -3642,19 +4079,19 @@
         <v>268778598.18300003</v>
       </c>
       <c r="V49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>268.77859818300004</v>
       </c>
       <c r="W49">
         <v>1.2553772966399999E-2</v>
       </c>
     </row>
-    <row r="50" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I50">
         <v>106787951.78</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>106.78795178</v>
       </c>
       <c r="K50">
@@ -3664,7 +4101,7 @@
         <v>119957224.13</v>
       </c>
       <c r="P50" s="1">
-        <f>O50/1000000</f>
+        <f t="shared" si="4"/>
         <v>119.95722413</v>
       </c>
       <c r="Q50">
@@ -3674,19 +4111,19 @@
         <v>269292343.62599999</v>
       </c>
       <c r="V50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>269.29234362599999</v>
       </c>
       <c r="W50">
         <v>1.3049559406700001E-2</v>
       </c>
     </row>
-    <row r="51" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I51">
         <v>108256429.455</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108.256429455</v>
       </c>
       <c r="K51">
@@ -3696,7 +4133,7 @@
         <v>120701639.978</v>
       </c>
       <c r="P51" s="1">
-        <f>O51/1000000</f>
+        <f t="shared" si="4"/>
         <v>120.701639978</v>
       </c>
       <c r="Q51">
@@ -3706,19 +4143,19 @@
         <v>269793426.074</v>
       </c>
       <c r="V51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>269.79342607400002</v>
       </c>
       <c r="W51">
         <v>1.35450910924E-2</v>
       </c>
     </row>
-    <row r="52" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I52">
         <v>109713160.76199999</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109.713160762</v>
       </c>
       <c r="K52">
@@ -3728,7 +4165,7 @@
         <v>121447538.892</v>
       </c>
       <c r="P52" s="1">
-        <f>O52/1000000</f>
+        <f t="shared" si="4"/>
         <v>121.44753889200001</v>
       </c>
       <c r="Q52">
@@ -3738,19 +4175,19 @@
         <v>270284048.47799999</v>
       </c>
       <c r="V52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>270.28404847799999</v>
       </c>
       <c r="W52">
         <v>1.4040366335900001E-2</v>
       </c>
     </row>
-    <row r="53" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="53" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I53">
         <v>111158527.20900001</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>111.15852720900001</v>
       </c>
       <c r="K53">
@@ -3760,7 +4197,7 @@
         <v>122194440.454</v>
       </c>
       <c r="P53" s="1">
-        <f>O53/1000000</f>
+        <f t="shared" si="4"/>
         <v>122.194440454</v>
       </c>
       <c r="Q53">
@@ -3770,19 +4207,19 @@
         <v>270765917.55900002</v>
       </c>
       <c r="V53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>270.765917559</v>
       </c>
       <c r="W53">
         <v>1.45353842418E-2</v>
       </c>
     </row>
-    <row r="54" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="54" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I54">
         <v>112592879.962</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112.592879962</v>
       </c>
       <c r="K54">
@@ -3792,7 +4229,7 @@
         <v>122941921.153</v>
       </c>
       <c r="P54" s="1">
-        <f>O54/1000000</f>
+        <f t="shared" si="4"/>
         <v>122.941921153</v>
       </c>
       <c r="Q54">
@@ -3802,19 +4239,19 @@
         <v>271240363.03500003</v>
       </c>
       <c r="V54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>271.24036303500003</v>
       </c>
       <c r="W54">
         <v>1.5030144483E-2</v>
       </c>
     </row>
-    <row r="55" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I55">
         <v>114016555.661</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>114.016555661</v>
       </c>
       <c r="K55">
@@ -3824,7 +4261,7 @@
         <v>123689607.858</v>
       </c>
       <c r="P55" s="1">
-        <f>O55/1000000</f>
+        <f t="shared" si="4"/>
         <v>123.689607858</v>
       </c>
       <c r="Q55">
@@ -3834,19 +4271,19 @@
         <v>271708427.74299997</v>
       </c>
       <c r="V55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>271.70842774299996</v>
       </c>
       <c r="W55">
         <v>1.5524647125999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="56" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I56">
         <v>115429860.079</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115.42986007899999</v>
       </c>
       <c r="K56">
@@ -3856,7 +4293,7 @@
         <v>124437170.66500001</v>
       </c>
       <c r="P56" s="1">
-        <f>O56/1000000</f>
+        <f t="shared" si="4"/>
         <v>124.43717066500001</v>
       </c>
       <c r="Q56">
@@ -3866,19 +4303,19 @@
         <v>272170930.22000003</v>
       </c>
       <c r="V56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>272.17093022</v>
       </c>
       <c r="W56">
         <v>1.6018892512000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="57" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I57">
         <v>116833088.152</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116.833088152</v>
       </c>
       <c r="K57">
@@ -3888,7 +4325,7 @@
         <v>125184319.854</v>
       </c>
       <c r="P57" s="1">
-        <f>O57/1000000</f>
+        <f t="shared" si="4"/>
         <v>125.18431985400001</v>
       </c>
       <c r="Q57">
@@ -3898,19 +4335,19 @@
         <v>272628512.954</v>
       </c>
       <c r="V57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>272.62851295399997</v>
       </c>
       <c r="W57">
         <v>1.65128811625E-2</v>
       </c>
     </row>
-    <row r="58" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="58" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I58">
         <v>137477357.83399999</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>137.477357834</v>
       </c>
       <c r="K58">
@@ -3920,7 +4357,7 @@
         <v>136585263.77700001</v>
       </c>
       <c r="P58" s="1">
-        <f>O58/1000000</f>
+        <f t="shared" si="4"/>
         <v>136.58526377700002</v>
       </c>
       <c r="Q58">
@@ -3930,19 +4367,19 @@
         <v>279283521.60399997</v>
       </c>
       <c r="V58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>279.28352160399999</v>
       </c>
       <c r="W58">
         <v>2.4137405794300001E-2</v>
       </c>
     </row>
-    <row r="59" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="59" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I59">
         <v>156466258.98899999</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>156.46625898899998</v>
       </c>
       <c r="K59">
@@ -3952,7 +4389,7 @@
         <v>147471045.79300001</v>
       </c>
       <c r="P59" s="1">
-        <f>O59/1000000</f>
+        <f t="shared" si="4"/>
         <v>147.471045793</v>
       </c>
       <c r="Q59">
@@ -3962,19 +4399,19 @@
         <v>285246243.47399998</v>
       </c>
       <c r="V59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>285.24624347399998</v>
       </c>
       <c r="W59">
         <v>3.1702928852200003E-2</v>
       </c>
     </row>
-    <row r="60" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="60" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I60">
         <v>174201782.83000001</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>174.20178283000001</v>
       </c>
       <c r="K60">
@@ -3984,7 +4421,7 @@
         <v>157810346.63100001</v>
       </c>
       <c r="P60" s="1">
-        <f>O60/1000000</f>
+        <f t="shared" si="4"/>
         <v>157.81034663100002</v>
       </c>
       <c r="Q60">
@@ -3994,19 +4431,19 @@
         <v>290524294.56400001</v>
       </c>
       <c r="V60" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>290.524294564</v>
       </c>
       <c r="W60">
         <v>3.9211168744100001E-2</v>
       </c>
     </row>
-    <row r="61" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="61" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I61">
         <v>190925336.22499999</v>
       </c>
       <c r="J61" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190.925336225</v>
       </c>
       <c r="K61">
@@ -4016,7 +4453,7 @@
         <v>167651266.002</v>
       </c>
       <c r="P61" s="1">
-        <f>O61/1000000</f>
+        <f t="shared" si="4"/>
         <v>167.651266002</v>
       </c>
       <c r="Q61">
@@ -4026,19 +4463,19 @@
         <v>295157996.60900003</v>
       </c>
       <c r="V61" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>295.15799660900001</v>
       </c>
       <c r="W61">
         <v>4.6663290104100003E-2</v>
       </c>
     </row>
-    <row r="62" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="62" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I62">
         <v>206795916.803</v>
       </c>
       <c r="J62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>206.79591680300001</v>
       </c>
       <c r="K62">
@@ -4048,7 +4485,7 @@
         <v>177049668.78400001</v>
       </c>
       <c r="P62" s="1">
-        <f>O62/1000000</f>
+        <f t="shared" si="4"/>
         <v>177.049668784</v>
       </c>
       <c r="Q62">
@@ -4058,19 +4495,19 @@
         <v>299219073.61400002</v>
       </c>
       <c r="V62" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>299.21907361400002</v>
       </c>
       <c r="W62">
         <v>5.4060221723100002E-2</v>
       </c>
     </row>
-    <row r="63" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="63" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I63">
         <v>221925774.91</v>
       </c>
       <c r="J63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>221.92577491</v>
       </c>
       <c r="K63">
@@ -4080,7 +4517,7 @@
         <v>186055133.20899999</v>
       </c>
       <c r="P63" s="1">
-        <f>O63/1000000</f>
+        <f t="shared" si="4"/>
         <v>186.05513320899999</v>
       </c>
       <c r="Q63">
@@ -4090,19 +4527,19 @@
         <v>302786689.39300001</v>
       </c>
       <c r="V63" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>302.78668939300002</v>
       </c>
       <c r="W63">
         <v>6.1402781437899998E-2</v>
       </c>
     </row>
-    <row r="64" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="64" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I64">
         <v>236396284.632</v>
       </c>
       <c r="J64" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>236.396284632</v>
       </c>
       <c r="K64">
@@ -4112,7 +4549,7 @@
         <v>194708945.14700001</v>
       </c>
       <c r="P64" s="1">
-        <f>O64/1000000</f>
+        <f t="shared" si="4"/>
         <v>194.70894514700001</v>
       </c>
       <c r="Q64">
@@ -4122,19 +4559,19 @@
         <v>305935866.97799999</v>
       </c>
       <c r="V64" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>305.93586697799998</v>
       </c>
       <c r="W64">
         <v>6.8691738022000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="65" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I65">
         <v>250266774.65000001</v>
       </c>
       <c r="J65" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>250.26677465</v>
       </c>
       <c r="K65">
@@ -4144,7 +4581,7 @@
         <v>203044667.96399999</v>
       </c>
       <c r="P65" s="1">
-        <f>O65/1000000</f>
+        <f t="shared" si="4"/>
         <v>203.04466796399998</v>
       </c>
       <c r="Q65">
@@ -4154,19 +4591,19 @@
         <v>308732522.00999999</v>
       </c>
       <c r="V65" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>308.73252200999997</v>
       </c>
       <c r="W65">
         <v>7.5927831717400002E-2</v>
       </c>
     </row>
-    <row r="66" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="66" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I66">
         <v>263585340.76899999</v>
       </c>
       <c r="J66" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>263.58534076899997</v>
       </c>
       <c r="K66">
@@ -4176,7 +4613,7 @@
         <v>211089653.54899999</v>
       </c>
       <c r="P66" s="1">
-        <f>O66/1000000</f>
+        <f t="shared" si="4"/>
         <v>211.08965354899999</v>
       </c>
       <c r="Q66">
@@ -4186,19 +4623,19 @@
         <v>311232549.85600001</v>
       </c>
       <c r="V66" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>311.23254985599999</v>
       </c>
       <c r="W66">
         <v>8.3111775421399997E-2</v>
       </c>
     </row>
-    <row r="67" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="67" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I67">
         <v>276392814.338</v>
       </c>
       <c r="J67" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>276.39281433799999</v>
       </c>
       <c r="K67">
@@ -4208,7 +4645,7 @@
         <v>218866499.99700001</v>
       </c>
       <c r="P67" s="1">
-        <f>O67/1000000</f>
+        <f t="shared" si="4"/>
         <v>218.86649999700001</v>
       </c>
       <c r="Q67">
@@ -4218,19 +4655,19 @@
         <v>313482494.73900002</v>
       </c>
       <c r="V67" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>313.482494739</v>
       </c>
       <c r="W67">
         <v>9.0244272020599994E-2</v>
       </c>
     </row>
-    <row r="68" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="68" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I68">
         <v>288721312.81300002</v>
       </c>
       <c r="J68" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>288.721312813</v>
       </c>
       <c r="K68">
@@ -4240,7 +4677,7 @@
         <v>226393688.81299999</v>
       </c>
       <c r="P68" s="1">
-        <f>O68/1000000</f>
+        <f t="shared" si="4"/>
         <v>226.39368881299998</v>
       </c>
       <c r="Q68">
@@ -4250,19 +4687,19 @@
         <v>315521066.49599999</v>
       </c>
       <c r="V68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>315.521066496</v>
       </c>
       <c r="W68">
         <v>9.7326023563400005E-2</v>
       </c>
     </row>
-    <row r="69" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="69" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I69">
         <v>300594894.54400003</v>
       </c>
       <c r="J69" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300.59489454400006</v>
       </c>
       <c r="K69">
@@ -4272,7 +4709,7 @@
         <v>233686797.22600001</v>
       </c>
       <c r="P69" s="1">
-        <f>O69/1000000</f>
+        <f t="shared" si="4"/>
         <v>233.68679722600001</v>
       </c>
       <c r="Q69">
@@ -4282,19 +4719,19 @@
         <v>317380721.56400001</v>
       </c>
       <c r="V69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>317.380721564</v>
       </c>
       <c r="W69">
         <v>0.104357715112</v>
       </c>
     </row>
-    <row r="70" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="70" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I70">
         <v>312040002.90100002</v>
       </c>
       <c r="J70" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>312.04000290100004</v>
       </c>
       <c r="K70">
@@ -4304,7 +4741,7 @@
         <v>240759775.102</v>
       </c>
       <c r="P70" s="1">
-        <f>O70/1000000</f>
+        <f t="shared" si="4"/>
         <v>240.75977510199999</v>
       </c>
       <c r="Q70">
@@ -4314,19 +4751,19 @@
         <v>319088520.463</v>
       </c>
       <c r="V70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>319.08852046300001</v>
       </c>
       <c r="W70">
         <v>0.111340011803</v>
       </c>
     </row>
-    <row r="71" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="71" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I71">
         <v>323075882.68400002</v>
       </c>
       <c r="J71" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>323.07588268400002</v>
       </c>
       <c r="K71">
@@ -4336,7 +4773,7 @@
         <v>247625098.36899999</v>
       </c>
       <c r="P71" s="1">
-        <f>O71/1000000</f>
+        <f t="shared" si="4"/>
         <v>247.625098369</v>
       </c>
       <c r="Q71">
@@ -4346,19 +4783,19 @@
         <v>320666999.40100002</v>
       </c>
       <c r="V71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>320.666999401</v>
       </c>
       <c r="W71">
         <v>0.118273580433</v>
       </c>
     </row>
-    <row r="72" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="72" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I72">
         <v>333719252.44400001</v>
       </c>
       <c r="J72" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>333.71925244400001</v>
       </c>
       <c r="K72">
@@ -4368,7 +4805,7 @@
         <v>254293792.80899999</v>
       </c>
       <c r="P72" s="1">
-        <f>O72/1000000</f>
+        <f t="shared" si="4"/>
         <v>254.293792809</v>
       </c>
       <c r="Q72">
@@ -4378,19 +4815,19 @@
         <v>322134530.36299998</v>
       </c>
       <c r="V72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>322.13453036299995</v>
       </c>
       <c r="W72">
         <v>0.12515909301200001</v>
       </c>
     </row>
-    <row r="73" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="73" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I73">
         <v>343990436.58700001</v>
       </c>
       <c r="J73" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>343.99043658700003</v>
       </c>
       <c r="K73">
@@ -4400,7 +4837,7 @@
         <v>260775322.352</v>
       </c>
       <c r="P73" s="1">
-        <f>O73/1000000</f>
+        <f t="shared" si="4"/>
         <v>260.77532235199999</v>
       </c>
       <c r="Q73">
@@ -4410,19 +4847,19 @@
         <v>323506044.67799997</v>
       </c>
       <c r="V73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>323.50604467799997</v>
       </c>
       <c r="W73">
         <v>0.13199721585099999</v>
       </c>
     </row>
-    <row r="74" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="74" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I74">
         <v>353904579.82099998</v>
       </c>
       <c r="J74" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>353.90457982099997</v>
       </c>
       <c r="K74">
@@ -4432,7 +4869,7 @@
         <v>267077688.49200001</v>
       </c>
       <c r="P74" s="1">
-        <f>O74/1000000</f>
+        <f t="shared" si="4"/>
         <v>267.07768849199999</v>
       </c>
       <c r="Q74">
@@ -4442,19 +4879,19 @@
         <v>324793753.61699998</v>
       </c>
       <c r="V74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>324.79375361699999</v>
       </c>
       <c r="W74">
         <v>0.13878860072999999</v>
       </c>
     </row>
-    <row r="75" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="75" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I75">
         <v>363476992.20499998</v>
       </c>
       <c r="J75" s="1">
-        <f t="shared" ref="J75:J83" si="4">I75/1000000</f>
+        <f t="shared" ref="J75:J83" si="6">I75/1000000</f>
         <v>363.47699220499999</v>
       </c>
       <c r="K75">
@@ -4464,7 +4901,7 @@
         <v>273207778.28399998</v>
       </c>
       <c r="P75" s="1">
-        <f>O75/1000000</f>
+        <f t="shared" ref="P75:P83" si="7">O75/1000000</f>
         <v>273.20777828399997</v>
       </c>
       <c r="Q75">
@@ -4474,19 +4911,19 @@
         <v>326007639.24599999</v>
       </c>
       <c r="V75" s="1">
-        <f t="shared" ref="V75:V83" si="5">U75/1000000</f>
+        <f t="shared" ref="V75:V83" si="8">U75/1000000</f>
         <v>326.007639246</v>
       </c>
       <c r="W75">
         <v>0.145533882413</v>
       </c>
     </row>
-    <row r="76" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="76" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I76">
         <v>372723850.09600002</v>
       </c>
       <c r="J76" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>372.72385009600004</v>
       </c>
       <c r="K76">
@@ -4496,7 +4933,7 @@
         <v>279172030.20099998</v>
       </c>
       <c r="P76" s="1">
-        <f>O76/1000000</f>
+        <f t="shared" si="7"/>
         <v>279.17203020099998</v>
       </c>
       <c r="Q76">
@@ -4506,19 +4943,19 @@
         <v>327155848.94</v>
       </c>
       <c r="V76" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>327.15584894</v>
       </c>
       <c r="W76">
         <v>0.152233682816</v>
       </c>
     </row>
-    <row r="77" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="77" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I77">
         <v>381657146.13499999</v>
       </c>
       <c r="J77" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>381.657146135</v>
       </c>
       <c r="K77">
@@ -4528,7 +4965,7 @@
         <v>284976220.94599998</v>
       </c>
       <c r="P77" s="1">
-        <f>O77/1000000</f>
+        <f t="shared" si="7"/>
         <v>284.97622094599996</v>
       </c>
       <c r="Q77">
@@ -4538,19 +4975,19 @@
         <v>328245182.19</v>
       </c>
       <c r="V77" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>328.24518218999998</v>
       </c>
       <c r="W77">
         <v>0.15888861288600001</v>
       </c>
     </row>
-    <row r="78" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="78" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I78">
         <v>387261375.454</v>
       </c>
       <c r="J78" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>387.26137545400002</v>
       </c>
       <c r="K78">
@@ -4560,7 +4997,7 @@
         <v>288638284.04900002</v>
       </c>
       <c r="P78" s="1">
-        <f>O78/1000000</f>
+        <f t="shared" si="7"/>
         <v>288.63828404900005</v>
       </c>
       <c r="Q78">
@@ -4570,19 +5007,19 @@
         <v>328919531.921</v>
       </c>
       <c r="V78" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>328.91953192099999</v>
       </c>
       <c r="W78">
         <v>0.16315858870399999</v>
       </c>
     </row>
-    <row r="79" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="79" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I79">
         <v>392743786.09399998</v>
       </c>
       <c r="J79" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>392.74378609399997</v>
       </c>
       <c r="K79">
@@ -4592,7 +5029,7 @@
         <v>292237117.34200001</v>
       </c>
       <c r="P79" s="1">
-        <f>O79/1000000</f>
+        <f t="shared" si="7"/>
         <v>292.23711734200003</v>
       </c>
       <c r="Q79">
@@ -4602,19 +5039,19 @@
         <v>329573485.27700001</v>
       </c>
       <c r="V79" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>329.57348527700003</v>
       </c>
       <c r="W79">
         <v>0.16741029443300001</v>
       </c>
     </row>
-    <row r="80" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="80" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I80">
         <v>398107289.44800001</v>
       </c>
       <c r="J80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>398.10728944800002</v>
       </c>
       <c r="K80">
@@ -4624,7 +5061,7 @@
         <v>295773878.62400001</v>
       </c>
       <c r="P80" s="1">
-        <f>O80/1000000</f>
+        <f t="shared" si="7"/>
         <v>295.77387862400002</v>
       </c>
       <c r="Q80">
@@ -4634,19 +5071,19 @@
         <v>330208173.75999999</v>
       </c>
       <c r="V80" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>330.20817375999997</v>
       </c>
       <c r="W80">
         <v>0.17164389030400001</v>
       </c>
     </row>
-    <row r="81" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I81">
         <v>403354269.58499998</v>
       </c>
       <c r="J81" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>403.354269585</v>
       </c>
       <c r="K81">
@@ -4656,7 +5093,7 @@
         <v>299249904.91000003</v>
       </c>
       <c r="P81" s="1">
-        <f>O81/1000000</f>
+        <f t="shared" si="7"/>
         <v>299.24990491</v>
       </c>
       <c r="Q81">
@@ -4666,19 +5103,19 @@
         <v>330824824.35100001</v>
       </c>
       <c r="V81" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>330.82482435100002</v>
       </c>
       <c r="W81">
         <v>0.175859532786</v>
       </c>
     </row>
-    <row r="82" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="82" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I82">
         <v>408488771.59600002</v>
       </c>
       <c r="J82" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>408.48877159599999</v>
       </c>
       <c r="K82">
@@ -4688,7 +5125,7 @@
         <v>302666465.00199997</v>
       </c>
       <c r="P82" s="1">
-        <f>O82/1000000</f>
+        <f t="shared" si="7"/>
         <v>302.666465002</v>
       </c>
       <c r="Q82">
@@ -4698,19 +5135,19 @@
         <v>331424601.76899999</v>
       </c>
       <c r="V82" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>331.42460176899999</v>
       </c>
       <c r="W82">
         <v>0.18005737689599999</v>
       </c>
     </row>
-    <row r="83" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="83" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I83">
         <v>413514421.685</v>
       </c>
       <c r="J83" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>413.514421685</v>
       </c>
       <c r="K83">
@@ -4720,7 +5157,7 @@
         <v>306024684.60900003</v>
       </c>
       <c r="P83" s="1">
-        <f>O83/1000000</f>
+        <f t="shared" si="7"/>
         <v>306.02468460900002</v>
       </c>
       <c r="Q83">
@@ -4730,7 +5167,7 @@
         <v>332008599.65100002</v>
       </c>
       <c r="V83" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>332.008599651</v>
       </c>
       <c r="W83">
@@ -4738,6 +5175,17 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="AB21:AC21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>